<commit_message>
Changes to PMs and documentation
</commit_message>
<xml_diff>
--- a/Outputs/OM_Design.xlsx
+++ b/Outputs/OM_Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\abft-mse\Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\abft-mse\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -194,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +372,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -555,9 +561,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -565,6 +570,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -888,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,534 +908,534 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="2:5" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="2:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+    <row r="3" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="5" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+    <row r="6" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+    <row r="9" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+    <row r="12" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="13" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
         <v>12</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C14" s="5">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+    <row r="15" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="16" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
+    <row r="18" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="19" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
         <v>18</v>
       </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="5">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+    <row r="21" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
         <v>19</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+    <row r="22" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23">
+    <row r="23" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
+    <row r="24" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <v>1</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25">
+    <row r="25" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>2</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26">
+    <row r="26" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
         <v>24</v>
       </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="5">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
+    <row r="27" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
         <v>25</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="28" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="29" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
         <v>27</v>
       </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="5">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+    <row r="30" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31">
+    <row r="31" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32">
+    <row r="32" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
         <v>30</v>
       </c>
-      <c r="C32">
-        <v>3</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="C32" s="5">
+        <v>3</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
+    <row r="33" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
         <v>31</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <v>1</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="34" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="35" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
         <v>33</v>
       </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1">
+    <row r="36" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
         <v>34</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <v>1</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="37" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
         <v>35</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="5">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="38" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
         <v>36</v>
       </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="5">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+    <row r="39" spans="2:5" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>